<commit_message>
EPBDS-8162 Make keyword "RETURN" optional for Spreadsheet tables that returns a particular type. Support transponsed tables.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8162_RETURN.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8162_RETURN.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747BFC71-5B8F-4310-8B2B-692D771540D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="13545" windowWidth="27795" xWindow="480" yWindow="180"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="94">
   <si>
     <t xml:space="preserve">Steps </t>
   </si>
@@ -270,12 +276,6 @@
     <t>Test mySpr_myDatatype_R1_ATFalse</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
     <t>properties</t>
   </si>
   <si>
@@ -285,38 +285,48 @@
     <t>RETURN1 : Double</t>
   </si>
   <si>
-    <t>=new  myDatatype ("test", 0)</t>
-  </si>
-  <si>
-    <t>_res_.$Value$Step2</t>
-  </si>
-  <si>
-    <t>_res_.$Value$RETURN1</t>
-  </si>
-  <si>
-    <t>_res_.$Value$Return1.$Value$Step1</t>
-  </si>
-  <si>
-    <t>_res_.$Value$RETURN1.$Value$Step2</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>=new  myDatatype ("test", 1)</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Spreadsheet DoubleValue mySprTrans (String param)</t>
+  </si>
+  <si>
+    <t>= $Value3</t>
+  </si>
+  <si>
+    <t>Test mySprTrans</t>
+  </si>
+  <si>
+    <t>param</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="000000" theme="1"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,6 +335,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,7 +370,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -432,110 +467,189 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
     <border>
-      <left style="thin"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
-    </border>
-    <border/>
-    <border>
-      <left style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
-    </border>
-    <border/>
-    <border>
-      <left style="thin"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
-    </border>
-    <border/>
-    <border>
-      <left style="thin"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
-    </border>
-    <border/>
-    <border>
-      <left style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17"/>
   </cellStyleXfs>
   <cellXfs count="47">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="10" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="13" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="14" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" borderId="16" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="true"/>
-    <xf borderId="19" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="true"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="true"/>
-    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="true"/>
-    <xf borderId="22" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="true"/>
-    <xf applyAlignment="1" applyBorder="true" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="true" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal 2 9" xfId="6" xr:uid="{16582FD7-D20E-44FA-857B-B28B380A3F2B}"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{966B3DE9-82D3-48A4-8929-9DCA4B42CBDE}"/>
+    <cellStyle name="Normal 3 2 2" xfId="5" xr:uid="{B2AB2A07-23B0-47E4-A374-A0B5EF71572B}"/>
+    <cellStyle name="Normal 6" xfId="2" xr:uid="{6DC51E2A-1D31-41B7-8D27-FBE7FA0730AD}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{80CBF67D-106D-425D-BA24-340D83F12172}"/>
+    <cellStyle name="Обычный 4" xfId="4" xr:uid="{CD8AFFB0-E9CC-414A-A712-B122F5B2AA60}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -561,29 +675,32 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -616,9 +733,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -651,9 +768,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,9 +820,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -741,7 +892,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -750,13 +901,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -766,7 +917,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -775,7 +926,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -784,7 +935,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -794,12 +945,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -830,7 +981,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -849,7 +1000,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -861,67 +1012,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="P68" sqref="P68"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="35.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="35.85546875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="68.42578125" collapsed="true"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.85546875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="68.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.5" r="2" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="H2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="M2" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="H5" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="M5" s="7" t="s">
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="M5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -948,16 +1100,16 @@
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="16" t="s">
-        <v>86</v>
+      <c r="M6" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="N6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O6" s="17" t="b">
+        <v>85</v>
+      </c>
+      <c r="O6" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="P6" s="18"/>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -997,7 +1149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1009,25 +1161,25 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9">
-      <c r="M9" s="15"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="12"/>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M9" s="11"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="H10" s="7" t="s">
+      <c r="C10" s="42"/>
+      <c r="H10" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="M10" s="7" t="s">
+      <c r="I10" s="42"/>
+      <c r="M10" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="7"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -1089,8 +1241,8 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.75" r="15" spans="2:16" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="16" spans="2:16" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>70</v>
       </c>
@@ -1109,24 +1261,24 @@
       <c r="P16" s="6"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="H19" s="9" t="s">
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="H19" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="11"/>
-      <c r="M19" s="9" t="s">
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45"/>
+      <c r="M19" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="11"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="45"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -1153,16 +1305,16 @@
       <c r="K20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M20" s="23" t="s">
-        <v>86</v>
+      <c r="M20" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="N20" t="s">
-        <v>87</v>
-      </c>
-      <c r="O20" s="24" t="b">
+        <v>85</v>
+      </c>
+      <c r="O20" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="P20" s="25"/>
+      <c r="P20" s="21"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -1202,7 +1354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1214,30 +1366,30 @@
       </c>
       <c r="P22" s="2"/>
     </row>
-    <row r="23">
-      <c r="M23" s="22"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="19"/>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M23" s="18"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="15"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="H24" s="7" t="s">
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="H24" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="M24" s="7" t="s">
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="M24" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="7"/>
-      <c r="O24" s="46"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="40"/>
       <c r="P24" s="7"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -1328,12 +1480,12 @@
       <c r="M27" s="1">
         <v>10</v>
       </c>
-      <c r="N27" s="1" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row ht="15.75" r="29" spans="2:16" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="30" spans="2:16" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>71</v>
       </c>
@@ -1352,24 +1504,24 @@
       <c r="P30" s="6"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
-      <c r="H33" s="9" t="s">
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+      <c r="H33" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="11"/>
-      <c r="M33" s="9" t="s">
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="45"/>
+      <c r="M33" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="11"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="45"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
@@ -1396,16 +1548,16 @@
       <c r="K34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M34" s="30" t="s">
-        <v>86</v>
+      <c r="M34" s="26" t="s">
+        <v>84</v>
       </c>
       <c r="N34" t="s">
-        <v>87</v>
-      </c>
-      <c r="O34" s="31" t="b">
+        <v>85</v>
+      </c>
+      <c r="O34" s="27" t="b">
         <v>0</v>
       </c>
-      <c r="P34" s="32"/>
+      <c r="P34" s="28"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -1445,9 +1597,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M36" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>4</v>
@@ -1457,30 +1609,30 @@
       </c>
       <c r="P36" s="2"/>
     </row>
-    <row r="37">
-      <c r="M37" s="29"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="26"/>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M37" s="25"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="22"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="H38" s="7" t="s">
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="H38" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="M38" s="7" t="s">
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="M38" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="42"/>
       <c r="P38" s="7"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -1588,8 +1740,8 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.75" r="43" spans="1:16" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="44" spans="1:16" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
         <v>69</v>
@@ -1709,22 +1861,22 @@
       <c r="N51" s="3"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="H53" s="7" t="s">
+      <c r="C53" s="42"/>
+      <c r="H53" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="I53" s="7"/>
-      <c r="J53" s="45"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="39"/>
       <c r="K53" s="7"/>
-      <c r="M53" s="7" t="s">
+      <c r="M53" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
@@ -1831,10 +1983,10 @@
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="7"/>
+      <c r="C60" s="42"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
@@ -1852,16 +2004,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25"/>
-    <row r="64"/>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="34"/>
-      <c r="O65" s="33"/>
+      <c r="M65" s="31"/>
+      <c r="N65" s="30"/>
+      <c r="O65" s="29"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
@@ -1878,11 +2028,11 @@
       <c r="C67" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M67" s="7" t="s">
+      <c r="M67" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="42"/>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M68" s="1" t="s">
@@ -1895,7 +2045,7 @@
         <v>68</v>
       </c>
     </row>
-    <row ht="15.75" r="69" spans="2:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M69" s="1" t="s">
         <v>6</v>
       </c>
@@ -1906,7 +2056,7 @@
         <v>68</v>
       </c>
     </row>
-    <row ht="15.75" r="70" spans="2:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4" t="s">
         <v>72</v>
       </c>
@@ -1920,13 +2070,13 @@
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
       <c r="M70" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O70" s="1" t="n">
-        <v>1.0</v>
+      <c r="O70" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
@@ -2035,16 +2185,16 @@
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
-      <c r="I83" s="7" t="s">
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="I83" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
+      <c r="J83" s="42"/>
+      <c r="K83" s="42"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
@@ -2106,27 +2256,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88">
-      <c r="B88" s="1" t="s">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-    </row>
-    <row r="89">
-      <c r="B89" s="42" t="s">
-        <v>86</v>
+      <c r="C88" s="46"/>
+      <c r="D88" s="46"/>
+      <c r="E88" s="46"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="36" t="s">
+        <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>87</v>
-      </c>
-      <c r="D89" s="43" t="b">
+        <v>85</v>
+      </c>
+      <c r="D89" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="E89" s="44"/>
-    </row>
-    <row r="90">
+      <c r="E89" s="38"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>33</v>
       </c>
@@ -2140,7 +2290,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>28</v>
       </c>
@@ -2150,36 +2300,147 @@
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92">
-      <c r="B92" t="s" s="1">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" t="s" s="2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="B93" s="41"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="38"/>
+      <c r="E92" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="35"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="32"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K97" s="35"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K98" s="35"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B99" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C99" s="46"/>
+      <c r="D99" s="46"/>
+      <c r="E99" s="46"/>
+      <c r="F99" s="1"/>
+      <c r="I99" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="J99" s="45"/>
+      <c r="K99" s="35"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B100" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D100" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E100" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K100" s="35"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C101" s="1">
+        <v>3</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K101" s="35"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1">
+        <v>2</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I102" s="1">
+        <v>1</v>
+      </c>
+      <c r="J102" s="1">
+        <v>2</v>
+      </c>
+      <c r="K102" s="35"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="K103" s="35"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K104" s="35"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K105" s="35"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K106" s="35"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K107" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="31">
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="I99:J99"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="I83:K83"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H38:K38"/>
     <mergeCell ref="M67:O67"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B38:E38"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="M33:P33"/>
     <mergeCell ref="M53:P53"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="I83:K83"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B33:E33"/>
@@ -2191,38 +2452,37 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="H24:K24"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="M33:P33"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>